<commit_message>
fix simple_selenium in tender
</commit_message>
<xml_diff>
--- a/data/tenders.xlsx
+++ b/data/tenders.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,243 +451,216 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Услуги</t>
+          <t>Услуги по перезарядке и ремонту огнетушителей, согласно технического задания (приложение 1 к государственному контракту)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01:59:36</t>
+          <t>01:27:03</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ФКУ "ЦОКР"</t>
+          <t>ФКУ ИК-6 УФСИН РОССИИ ПО Г. САНКТ-ПЕТЕРБУРГУ И ЛЕНИНГРАДСКОЙ ОБЛАСТИ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>231 600,00 руб.</t>
+          <t>66 183,43 руб.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386994/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1392493/order-info</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>перезарядка огнетушителей, 7 усл. ед</t>
+          <t>Заправка огнетушителей, 4 шт</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>01:58:52</t>
+          <t>01:14:23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Филиал - 3 отряд ФКУ "ГУ "ВО Минфина России"</t>
+          <t>ОТДЕЛ МВД РОССИИ ПО ИГЛИНСКОМУ РАЙОНУ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1 000,00 руб.</t>
+          <t>840,00 руб.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386846/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1392389/order-info</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Услуги по техническому обслуживанию,зарядке и ремонту огнетушителей, 40 усл. ед</t>
+          <t>Переосвидетельствование и перезарядка огнетушителей., 30 шт</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>01:58:52</t>
+          <t>23:01:43</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ОМВД РОССИИ ПО СЛЮДЯНСКОМУ РАЙОНУ</t>
+          <t>ОМВД РОССИИ ПО КАМЫЗЯКСКОМУ РАЙОНУ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>6 000,00 руб.</t>
+          <t>3 600,00 руб.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386622/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1392302/order-info</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Приобретение продукции для обеспечения пожарной безопасности</t>
+          <t>Перезарядка огнетушителя ОП-2, 4 шт</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01:58:03</t>
+          <t>22:18:04</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ФКУ ИК-4 УФСИН РОССИИ ПО КУРГАНСКОЙ ОБЛАСТИ</t>
+          <t>ОТДЕЛ ГФС РОССИИ В Г. ВЕЛИКОМ НОВГОРОДЕ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>19 250,00 руб.</t>
+          <t>1 900,00 руб.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386487/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1392001/order-info</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Техническое обслуживание огнетушителей, 1 шт</t>
+          <t>Одежда и обувь, Автомобильные товары и запчасти</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23:57:58</t>
+          <t>20:42:01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ГУ "ОТДЕЛ МВД РОССИИ ПО ЯКШУР-БОДЬИНСКОМУ РАЙОНУ"</t>
+          <t>ФКУКИИ "КУЛЬТУРНЫЙ ЦЕНТР МВД РОССИИ"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3 600,00 руб.</t>
+          <t>7 500,00 руб.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386448/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1391454/order-info</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Услуги по техническому обслуживанию огнетушителей,(согласно приложенному техническому заданию)- 16 шт</t>
+          <t>Оказание услуг по вывозу и утилизации огнетушителей, 1 усл. ед</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01:57:41</t>
+          <t>17:19:56</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ФГКУ КОМБИНАТ "НОВЫЙ ПУТЬ" РОСРЕЗЕРВА</t>
+          <t>УТ МВД РОССИИ ПО ДФО</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4 780,00 руб.</t>
+          <t>29 200,00 руб.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1386332/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1389772/order-info</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ПЕРЕЗАРЯДКА ОГНЕТУШИТЕЛЕЙ, 1 шт</t>
+          <t>Выполнение работ по техническому обслуживанию углекислотных огнетушителей, 300 шт</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01:57:12</t>
+          <t>01:39:34</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ОМВД РОССИИ ПО КАРАЧЕВСКОМУ РАЙОНУ</t>
+          <t>ФСО РОССИИ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7 750,00 руб.</t>
+          <t>195 000,00 руб.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1385769/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1388261/order-info</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Оказание услуг по заправке огнетушителей ОУ-5</t>
+          <t>Техническое обслуживание и перезарядка огнетушителей, 132 шт</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>01:56:48</t>
+          <t>01:01:09</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ФГКУ "ЦЕНТРРЕЗЕРВ"</t>
+          <t>ФГКУ КОМБИНАТ "СИГНАЛ" ИМ. А.А. ГРИГОРЬЕВА РОСРЕЗЕРВА</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7 995,00 руб.</t>
+          <t>95 850,00 руб.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://agregatoreat.ru/purchase/1383708/order-info</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>На поставку огнетушителей</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>01:56:31</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>ГЛАВНОЕ УПРАВЛЕНИЕ МЧС РОССИИ ПО ТЮМЕНСКОЙ ОБЛАСТИ</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>100 000,00 руб.</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://agregatoreat.ru/purchase/1382940/order-info</t>
+          <t>https://agregatoreat.ru/purchase/1388110/order-info</t>
         </is>
       </c>
     </row>

</xml_diff>